<commit_message>
cases index bug fix
</commit_message>
<xml_diff>
--- a/process.xlsx
+++ b/process.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ikopryakov/Documents/GitHub/as-crew/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDBC5F74-08FF-7345-9486-E1CDC29C20FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{846EC294-8B76-EC42-98C3-9309C82514BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1540" windowWidth="28040" windowHeight="17360" xr2:uid="{6B8579EF-46A6-4546-8987-9DD378EDEA69}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Almette</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Popup Start a Project</t>
   </si>
   <si>
-    <t>Privacy Notice</t>
-  </si>
-  <si>
     <t>Pricing</t>
   </si>
   <si>
@@ -102,13 +99,13 @@
     <t>Пока не делаем</t>
   </si>
   <si>
-    <t>Ждем текст</t>
-  </si>
-  <si>
     <t>Доработка макета</t>
   </si>
   <si>
     <t>Нет макета</t>
+  </si>
+  <si>
+    <t>Privacy Police</t>
   </si>
 </sst>
 </file>
@@ -155,7 +152,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -186,12 +183,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -253,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -288,9 +279,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -662,7 +650,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="156" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -674,13 +662,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C1" s="11" t="s">
         <v>18</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -688,7 +676,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C2" s="7"/>
     </row>
@@ -753,7 +741,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C11" s="7"/>
     </row>
@@ -783,35 +771,33 @@
         <v>13</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C15" s="7"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>22</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B16" s="4"/>
       <c r="C16" s="7"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" s="7"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="13"/>
       <c r="C18" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>